<commit_message>
working on some stuff
</commit_message>
<xml_diff>
--- a/Main Assesment/Data/bb1a.xlsx
+++ b/Main Assesment/Data/bb1a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\as3122\Desktop\Isaac Newtron BB Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilsonporteus/Documents/GitHub/ssb_s5/Main Assesment/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FB78472-E7B9-4986-80B9-04E7F7BA20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B2671B-8D50-6149-AC37-26DB5100756D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C9F0040C-5813-487F-8842-8AE7237BED46}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19440" windowHeight="15000" xr2:uid="{C9F0040C-5813-487F-8842-8AE7237BED46}"/>
   </bookViews>
   <sheets>
     <sheet name="End point" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -625,773 +624,799 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF8E6DA-E0BE-4B19-9DCC-6E862A1CBA1A}">
   <dimension ref="A3:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>5</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>6</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>7</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>8</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>9</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>10</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <v>11</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <v>12</v>
       </c>
-      <c r="O14" s="13" t="s">
+      <c r="O14" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>2E-3</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>-5.1250000000000004E-4</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>-0.01</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>-8.1249999999999996E-4</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <v>-2.1999999999999999E-2</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="O15" s="14"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="M15" s="4"/>
+      <c r="O15" s="13"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>-2E-3</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>-2E-3</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>-1.125E-4</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="M16" s="8"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>0.01</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>7.8750000000000001E-4</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>-2.3E-2</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="M17" s="8"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>-2E-3</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>2E-3</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>1E-3</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <v>2E-3</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="6">
         <v>6.8749999999999996E-4</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="M18" s="8"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>-1E-3</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="6">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="M19" s="7"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <v>2E-3</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="6">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="M20" s="8"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="M20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="M21" s="8"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>0.01</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>0.01</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="9">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <v>2E-3</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="9">
         <v>1E-3</v>
       </c>
-      <c r="M22" s="11"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="10"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="O24" s="12"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+      <c r="O24" s="11"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>2</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>3</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>4</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>5</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>6</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>7</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>8</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <v>9</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>10</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="1">
         <v>11</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <v>12</v>
       </c>
-      <c r="O25" s="13" t="s">
+      <c r="O25" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <v>9.875000000000001E-4</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>-1E-3</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <v>-2E-3</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="3">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="3">
         <v>-2.4E-2</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="3">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="M26" s="5"/>
-      <c r="O26" s="14"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="M26" s="4"/>
+      <c r="O26" s="13"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="6">
         <v>2E-3</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L27" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="M27" s="8"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="M27" s="7"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>0.01</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="6">
         <v>-2.1999999999999999E-2</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L28" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="M28" s="8"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>-2.1249999999999999E-4</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>2E-3</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="6">
         <v>-2.1249999999999999E-4</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="6">
         <v>1E-3</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="6">
         <v>-1E-3</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="M29" s="8"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>1.2E-2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>-2E-3</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="6">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="M30" s="8"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="M30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>0.02</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="6">
         <v>9.875000000000001E-4</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="6">
         <v>1.875E-4</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="6">
         <v>-0.05</v>
       </c>
-      <c r="M31" s="8"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="M31" s="7"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>1.6E-2</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L32" s="7">
+      <c r="L32" s="6">
         <v>2E-3</v>
       </c>
-      <c r="M32" s="8"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="M32" s="7"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>1.2E-2</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="9">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="9">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="H33" s="10">
+      <c r="H33" s="9">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="9">
         <v>-1.2500000000000001E-5</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K33" s="9">
         <v>2E-3</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M33" s="11"/>
+      <c r="M33" s="10"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B15:L22">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:L33">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>